<commit_message>
I generated tablesfor all LRT in SA1
</commit_message>
<xml_diff>
--- a/practicum 2 Table 1 categorical variable counts.xlsx
+++ b/practicum 2 Table 1 categorical variable counts.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1480" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="5600" windowWidth="25600" windowHeight="15460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -501,7 +501,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="125" zoomScaleNormal="125" zoomScalePageLayoutView="125" workbookViewId="0">
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>

</xml_diff>